<commit_message>
smartthigns Thinq 분위기 안심 트렌드
</commit_message>
<xml_diff>
--- a/현황표.xlsx
+++ b/현황표.xlsx
@@ -453,6 +453,9 @@
       <c r="G2" t="str">
         <v>안심</v>
       </c>
+      <c r="H2" t="str">
+        <v>O</v>
+      </c>
       <c r="I2" t="str">
         <v>안방</v>
       </c>
@@ -479,6 +482,9 @@
       <c r="G3" t="str">
         <v>트렌드</v>
       </c>
+      <c r="H3" t="str">
+        <v>O</v>
+      </c>
       <c r="I3" t="str">
         <v>주발</v>
       </c>
@@ -497,13 +503,16 @@
         <v>서큘레이터</v>
       </c>
       <c r="D4" t="str">
-        <v>o</v>
+        <v>O</v>
       </c>
       <c r="E4" t="str">
         <v>분위기</v>
       </c>
       <c r="G4" t="str">
         <v>분위기</v>
+      </c>
+      <c r="H4" t="str">
+        <v>O</v>
       </c>
       <c r="I4" t="str">
         <v>거실</v>
@@ -523,13 +532,16 @@
         <v>음식</v>
       </c>
       <c r="D5" t="str">
-        <v>o</v>
+        <v>O</v>
       </c>
       <c r="E5" t="str">
         <v>낮잠</v>
       </c>
       <c r="G5" t="str">
         <v>Thinkq</v>
+      </c>
+      <c r="H5" t="str">
+        <v>O</v>
       </c>
       <c r="I5" t="str">
         <v>벽</v>
@@ -549,13 +561,16 @@
         <v>설치</v>
       </c>
       <c r="D6" t="str">
-        <v>ㅈㅣㄴ행중</v>
+        <v>O</v>
       </c>
       <c r="E6" t="str">
         <v>하교</v>
       </c>
       <c r="G6" t="str">
         <v>smartthings</v>
+      </c>
+      <c r="H6" t="str">
+        <v>O</v>
       </c>
       <c r="I6" t="str">
         <v>확장형</v>
@@ -575,7 +590,7 @@
         <v>외출</v>
       </c>
       <c r="D7" t="str">
-        <v>ㅈㄴ행중</v>
+        <v>O</v>
       </c>
       <c r="E7" t="str">
         <v>홈캉스</v>
@@ -597,6 +612,9 @@
       <c r="C8" t="str">
         <v>역류</v>
       </c>
+      <c r="D8" t="str">
+        <v>o</v>
+      </c>
       <c r="E8" t="str">
         <v>개학</v>
       </c>
@@ -614,6 +632,9 @@
       <c r="C9" t="str">
         <v>알레르기</v>
       </c>
+      <c r="D9" t="str">
+        <v>o</v>
+      </c>
       <c r="E9" t="str">
         <v>낮잠</v>
       </c>
@@ -630,6 +651,9 @@
       </c>
       <c r="C10" t="str">
         <v>씽큐</v>
+      </c>
+      <c r="D10" t="str">
+        <v>o</v>
       </c>
       <c r="E10" t="str">
         <v>알러지</v>

</xml_diff>